<commit_message>
Modificacion indice tentativo y creacion capitulo II
</commit_message>
<xml_diff>
--- a/TESIS/3. Marco Teórico/Indice tentativo.xlsx
+++ b/TESIS/3. Marco Teórico/Indice tentativo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aleksander\Documents\Universidad\1. Proyecto de graduación I\TESIS\3. Marco Teórico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3869AFAE-3B0B-445D-B18F-57B386C4BB05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7348FD-1D22-4794-A2EA-E412C95B67B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11310" xr2:uid="{E1B47254-E46F-4E91-966E-199DEFEE677F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="367">
   <si>
     <t>Tienda de Ropa Niche</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Incremento de ventas</t>
   </si>
   <si>
-    <t>Que es incremento</t>
-  </si>
-  <si>
     <t>Definición de incremento de ventas</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>Expansión de Mercado</t>
   </si>
   <si>
-    <t>https://diccionarioactual.com/expansion/</t>
-  </si>
-  <si>
     <t>https://economipedia.com/definiciones/mercado.html</t>
   </si>
   <si>
@@ -245,27 +239,9 @@
     <t>Que es publicidad</t>
   </si>
   <si>
-    <t>Publicidad exterior</t>
-  </si>
-  <si>
-    <t>Publicidad en vallas y carteleras</t>
-  </si>
-  <si>
-    <t>Publicidad en medios impresos y masivos</t>
-  </si>
-  <si>
-    <t>Publiciad directa</t>
-  </si>
-  <si>
-    <t>Publiciad de mano en mano</t>
-  </si>
-  <si>
     <t>Publicidad de boca en boca</t>
   </si>
   <si>
-    <t>Realizacion de promociones</t>
-  </si>
-  <si>
     <t>Definicion</t>
   </si>
   <si>
@@ -290,9 +266,6 @@
     <t>Catálogos</t>
   </si>
   <si>
-    <t>Publicidad tradicional</t>
-  </si>
-  <si>
     <t>Publicidad en internet</t>
   </si>
   <si>
@@ -1014,6 +987,156 @@
   </si>
   <si>
     <t>https://redhistoria.com/breve-historia-de-la-venta-y-los-vendedores/#:~:text=Podr%C3%ADa%20decirse%20que%20el%20origen,hac%C3%ADa%20falta%20con%20otros%20humanos.</t>
+  </si>
+  <si>
+    <t>https://www.gestiopolis.com/venta-directa-venta-indirecta-y-sistemas-de-distribucion-que-son/</t>
+  </si>
+  <si>
+    <t>https://elviajedelcliente.com/venta-cruzada-que-es/</t>
+  </si>
+  <si>
+    <t>No agregado</t>
+  </si>
+  <si>
+    <t>agregado</t>
+  </si>
+  <si>
+    <t>https://www.rdstation.com/es/blog/inbound-vs-outbound-sales/#:~:text=El%20Inbound%20sales%20(o%20ventas,enviados%20al%20equipo%20de%20ventas.</t>
+  </si>
+  <si>
+    <t>https://www.elsevier.es/es-revista-offarm-4-pdf-13102418</t>
+  </si>
+  <si>
+    <t>https://www.elsevier.es/es-revista-offarm-4-articulo-promocion-comunicacion-importancia-venta-personal-13102418#:~:text=La%20venta%20personal%20es%20un,oral%20entre%20vendedor%20y%20comprador.</t>
+  </si>
+  <si>
+    <t>https://rockcontent.com/es/blog/marketplace/</t>
+  </si>
+  <si>
+    <t>http://diposit.ub.edu/dspace/bitstream/2445/51104/1/memoria.pdf</t>
+  </si>
+  <si>
+    <t>pag16</t>
+  </si>
+  <si>
+    <t>https://es.shopify.com/blog/ecommerce-y-redes-sociales</t>
+  </si>
+  <si>
+    <t>https://blog.saleslayer.com/es/tipos-de-tienda-online</t>
+  </si>
+  <si>
+    <t>https://www.economiasimple.net/glosario/c2b</t>
+  </si>
+  <si>
+    <t>https://www.spri.eus/euskadinnova/es/enpresa-digitala/publicaciones/business-administration/1131.aspx</t>
+  </si>
+  <si>
+    <t>https://www.doofinder.com/es/blog/que-es-e-commerce</t>
+  </si>
+  <si>
+    <t>Definición de incremento</t>
+  </si>
+  <si>
+    <t>http://www.eco.uva.es/firmaelectronica/res/firma_electronica.pdf</t>
+  </si>
+  <si>
+    <t>Promociones de ventas</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/promocion-de-ventas.html</t>
+  </si>
+  <si>
+    <t>Formas de realizar promociones</t>
+  </si>
+  <si>
+    <t>Promocion en precio</t>
+  </si>
+  <si>
+    <t>Promocion en cantidad</t>
+  </si>
+  <si>
+    <t>Promocion en servicio posventa</t>
+  </si>
+  <si>
+    <t>Promocion de duracion</t>
+  </si>
+  <si>
+    <t>https://blog.citytroops.com/es/publicidad-en-lugar-de-venta/</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/bonificacion.html</t>
+  </si>
+  <si>
+    <t>https://www.promonegocios.net/oferta/definicion-oferta.html</t>
+  </si>
+  <si>
+    <t>https://www.merca20.com/que-son-las-muestras-promocionales-conoce-estos-7-tipos/</t>
+  </si>
+  <si>
+    <t>Tipos de Muestras</t>
+  </si>
+  <si>
+    <t>Muestra Cruzada</t>
+  </si>
+  <si>
+    <t>Muestra Directa</t>
+  </si>
+  <si>
+    <t>https://www.informabtl.com/que-es-una-promocion-cruzada-funcionan/#:~:text=Las%20practicas%20de%20promoci%C3%B3n%20cruzada&amp;text=Es%20cuando%20en%20las%20tiendas,otro%20marca%20que%20est%C3%A1%20aliado.&amp;text=Por%20ejemplo%20cuando%20se%20regalan,consume%20una%20marca%20en%20especial.</t>
+  </si>
+  <si>
+    <t>Muestra Distribuida en tienda</t>
+  </si>
+  <si>
+    <t>https://www.definicionabc.com/economia/expansion.php</t>
+  </si>
+  <si>
+    <t>Comprador</t>
+  </si>
+  <si>
+    <t>Vendedor</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/vendedor.html</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/comprador.html</t>
+  </si>
+  <si>
+    <t>https://www.bbva.es/finanzas-vistazo/ef/empresas/expansion-diversificacion.html</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/desarrollo-nuevo-producto.html</t>
+  </si>
+  <si>
+    <t>https://www.zendesk.com.mx/blog/desarrollo-de-mercado/#:~:text=desarrollo%20de%20mercado-,%C2%BFQu%C3%A9%20es%20desarrollo%20de%20mercado%3F,los%20que%20act%C3%BAa%20en%20general.</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/publicidad.html</t>
+  </si>
+  <si>
+    <t>Publicidad en televisión</t>
+  </si>
+  <si>
+    <t>https://www.redalyc.org/pdf/158/15825078.pdf</t>
+  </si>
+  <si>
+    <t>Publicidad en radio</t>
+  </si>
+  <si>
+    <t>https://zizer.es/blog/campanas-de-publicidad-en-radio-sector-salud/</t>
+  </si>
+  <si>
+    <t>Publicidad impresa</t>
+  </si>
+  <si>
+    <t>https://economipedia.com/definiciones/publicidad-impresa.html</t>
+  </si>
+  <si>
+    <t>https://rockcontent.com/es/blog/marketing-boca-a-boca/</t>
+  </si>
+  <si>
+    <t>https://www.cyberclick.es/que-es/publicidad-en-internet</t>
   </si>
 </sst>
 </file>
@@ -1053,12 +1176,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1074,7 +1209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1087,6 +1222,21 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1404,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92035BB4-4169-4D4D-BF97-B0E3E61C2DF1}">
-  <dimension ref="A1:S150"/>
+  <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F81" sqref="F81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,23 +1587,31 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
+      <c r="L2" s="10"/>
+      <c r="M2" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
+      <c r="L3" s="8"/>
+      <c r="M3" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1461,7 +1619,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D5" t="s">
         <v>2</v>
@@ -1469,7 +1627,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -1477,7 +1635,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1485,7 +1643,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
@@ -1493,7 +1651,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -1501,26 +1659,29 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
       <c r="B11" s="6" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="S11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -1530,102 +1691,162 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="6" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D13" t="s">
         <v>2</v>
       </c>
       <c r="J13" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E15" t="s">
         <v>19</v>
       </c>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
       <c r="J15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="6" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D18" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D18" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="6" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E19" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="6" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D23" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" t="s">
+        <v>322</v>
+      </c>
+      <c r="O22" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D23" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="D24" t="s">
         <v>28</v>
@@ -1634,1125 +1855,1450 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="E26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" t="s">
+        <v>325</v>
+      </c>
+      <c r="P27" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C28" s="6" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="6" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="E30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D30" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="E30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="E31" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E32" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
       <c r="D33" s="6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D34" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D34" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C35" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" t="s">
+        <v>332</v>
+      </c>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="D37" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" t="s">
+        <v>50</v>
+      </c>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="J43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D44" t="s">
+        <v>53</v>
+      </c>
+      <c r="J44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D36" t="s">
-        <v>42</v>
-      </c>
-      <c r="J36" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="D45" t="s">
+        <v>334</v>
+      </c>
+      <c r="J45" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="D46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C49" s="9"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C50" s="9"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C51" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" t="s">
+        <v>336</v>
+      </c>
+      <c r="J51" t="s">
         <v>43</v>
       </c>
-      <c r="J37" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C38" s="6" t="s">
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="D38" t="s">
-        <v>47</v>
-      </c>
-      <c r="J38" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C39" s="6" t="s">
+      <c r="E52" t="s">
+        <v>70</v>
+      </c>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="D39" t="s">
-        <v>49</v>
-      </c>
-      <c r="J39" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D40" s="6" t="s">
+      <c r="E53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I53" s="8"/>
+      <c r="J53" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E40" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D41" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="E41" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D42" s="6" t="s">
+      <c r="E55" t="s">
+        <v>73</v>
+      </c>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="12" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="12" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D60" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E42" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D43" s="6" t="s">
+      <c r="E60" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D61" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="E43" t="s">
-        <v>88</v>
-      </c>
-      <c r="J43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C44" s="6" t="s">
+      <c r="E61" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="D44" t="s">
-        <v>54</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="C62" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C45" s="6" t="s">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D45" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C46" s="6" t="s">
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D64" t="s">
+        <v>59</v>
+      </c>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" t="s">
+        <v>56</v>
+      </c>
+      <c r="O64" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="8"/>
+      <c r="E65" t="s">
+        <v>351</v>
+      </c>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="8"/>
+      <c r="E66" t="s">
+        <v>352</v>
+      </c>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C67" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D67" t="s">
+        <v>60</v>
+      </c>
+      <c r="J67" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C68" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C69" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="D69" t="s">
+        <v>83</v>
+      </c>
+      <c r="J69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="E70" t="s">
+        <v>62</v>
+      </c>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="E71" t="s">
+        <v>63</v>
+      </c>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="E72" t="s">
+        <v>64</v>
+      </c>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D73" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E73" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="D74" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="D75" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E75" t="s">
+        <v>359</v>
+      </c>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="D76" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E76" t="s">
+        <v>361</v>
+      </c>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E77" t="s">
+        <v>363</v>
+      </c>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="D78" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E78" t="s">
+        <v>67</v>
+      </c>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="E79" t="s">
+        <v>76</v>
+      </c>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D80" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D81" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D82" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="D83" t="s">
         <v>77</v>
       </c>
-      <c r="J46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D47" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="E47" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D84" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E84" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D85" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="E85" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="E48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D49" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E49" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D50" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="E50" t="s">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B86" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D51" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="E51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D52" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="E52" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="C53" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C54" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D54" t="s">
-        <v>60</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C55" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="D55" t="s">
-        <v>61</v>
-      </c>
-      <c r="J55" t="s">
-        <v>58</v>
-      </c>
-      <c r="O55" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C56" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D56" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C57" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="D57" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C58" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D58" t="s">
-        <v>92</v>
-      </c>
-      <c r="J58" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D59" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="E59" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D60" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="E60" t="s">
-        <v>65</v>
-      </c>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D61" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="E61" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D62" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E62" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C63" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" t="s">
-        <v>68</v>
-      </c>
-      <c r="J63" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="D64" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="E64" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D65" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="E65" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D66" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="E66" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D67" s="6" t="s">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="E67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D68" s="6" t="s">
+      <c r="C87" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="6"/>
+      <c r="C88" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="E68" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D69" s="6" t="s">
+      <c r="D88" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="E69" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D70" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E70" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D71" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="E71" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C72" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D72" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D73" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="E73" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D74" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="E74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="B75" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="C76" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="6"/>
-      <c r="C77" s="6" t="s">
-        <v>252</v>
-      </c>
-      <c r="D77" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="6" t="s">
-        <v>253</v>
-      </c>
-      <c r="C78" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="6"/>
-      <c r="C79" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="D79" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="C80" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B81" s="6"/>
-      <c r="C81" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="D81" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B82" s="6"/>
-      <c r="C82" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="D82" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="6"/>
-      <c r="D83" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E83" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B84" s="6"/>
-      <c r="D84" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="E84" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="6"/>
-      <c r="D85" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="E85" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B86" s="6"/>
-      <c r="D86" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="E86" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B87" s="6"/>
-      <c r="D87" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E87" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C88" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B89" s="6"/>
-      <c r="C89" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="C89" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B90" s="6"/>
       <c r="C90" s="6" t="s">
-        <v>265</v>
+        <v>245</v>
       </c>
       <c r="D90" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="C91" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="6"/>
+      <c r="C92" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="D92" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="6"/>
+      <c r="C93" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="D93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B91" s="6"/>
-      <c r="C91" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="D91" t="s">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="6"/>
+      <c r="D94" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="E94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="6"/>
+      <c r="D95" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E95" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="6"/>
-      <c r="D92" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="E92" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B93" s="6"/>
-      <c r="D93" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="E93" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B94" s="6"/>
-      <c r="C94" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D94" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="6"/>
-      <c r="C95" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D95" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C96" t="s">
-        <v>111</v>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="6"/>
+      <c r="D96" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E96" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B97" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="C97" t="s">
-        <v>118</v>
+      <c r="B97" s="6"/>
+      <c r="D97" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="E97" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="98" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B98" s="6"/>
-      <c r="C98" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D98" t="s">
-        <v>116</v>
+      <c r="D98" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E98" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="99" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B99" s="6"/>
-      <c r="C99" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="D99" t="s">
-        <v>117</v>
+      <c r="B99" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="C99" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B100" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="C100" t="s">
-        <v>121</v>
+      <c r="B100" s="6"/>
+      <c r="C100" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D100" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B101" s="6"/>
       <c r="C101" s="6" t="s">
-        <v>276</v>
+        <v>256</v>
       </c>
       <c r="D101" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B102" s="6"/>
-      <c r="D102" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="E102" t="s">
-        <v>124</v>
+      <c r="C102" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D102" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B103" s="6"/>
       <c r="D103" s="6" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="E103" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B104" s="6"/>
       <c r="D104" s="6" t="s">
-        <v>279</v>
+        <v>259</v>
       </c>
       <c r="E104" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="105" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B105" s="6"/>
-      <c r="D105" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="E105" t="s">
-        <v>127</v>
+      <c r="C105" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D105" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="106" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B106" s="6"/>
-      <c r="D106" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="E106" t="s">
-        <v>128</v>
+      <c r="C106" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D106" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="107" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B107" s="6"/>
-      <c r="D107" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="E107" t="s">
-        <v>129</v>
+      <c r="B107" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="C107" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="6"/>
-      <c r="C108" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="D108" t="s">
-        <v>122</v>
+      <c r="B108" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C108" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B109" s="6"/>
-      <c r="D109" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="E109" t="s">
-        <v>132</v>
+      <c r="C109" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="D109" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B110" s="6"/>
-      <c r="D110" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="E110" t="s">
-        <v>133</v>
+      <c r="C110" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="6"/>
-      <c r="D111" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="E111" t="s">
-        <v>134</v>
+      <c r="B111" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="C111" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="112" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B112" s="6"/>
-      <c r="D112" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="E112" t="s">
-        <v>135</v>
+      <c r="C112" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D112" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C113" t="s">
-        <v>139</v>
+      <c r="B113" s="6"/>
+      <c r="D113" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E113" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="6"/>
-      <c r="C114" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="D114" t="s">
-        <v>140</v>
+      <c r="D114" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="E114" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="6"/>
       <c r="D115" s="6" t="s">
-        <v>290</v>
+        <v>270</v>
       </c>
       <c r="E115" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="116" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B116" s="6"/>
       <c r="D116" s="6" t="s">
-        <v>291</v>
+        <v>271</v>
       </c>
       <c r="E116" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B117" s="6"/>
       <c r="D117" s="6" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="E117" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B118" s="6"/>
-      <c r="C118" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="D118" t="s">
-        <v>151</v>
+      <c r="D118" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="E118" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B119" s="6"/>
-      <c r="D119" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E119" t="s">
-        <v>145</v>
+      <c r="C119" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D119" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B120" s="6"/>
       <c r="D120" s="6" t="s">
-        <v>295</v>
+        <v>275</v>
       </c>
       <c r="E120" t="s">
-        <v>146</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B121" s="6"/>
       <c r="D121" s="6" t="s">
-        <v>296</v>
+        <v>276</v>
       </c>
       <c r="E121" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B122" s="6"/>
       <c r="D122" s="6" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="E122" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B123" s="6"/>
       <c r="D123" s="6" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="E123" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
     </row>
     <row r="124" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B124" s="6"/>
-      <c r="C124" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="D124" t="s">
-        <v>150</v>
+      <c r="B124" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C124" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B125" s="6"/>
-      <c r="D125" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="E125" t="s">
-        <v>152</v>
+      <c r="C125" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D125" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B126" s="6"/>
       <c r="D126" s="6" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="E126" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B127" s="6" t="s">
-        <v>302</v>
-      </c>
-      <c r="C127" t="s">
-        <v>158</v>
+      <c r="B127" s="6"/>
+      <c r="D127" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="E127" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B128" s="6"/>
-      <c r="C128" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="D128" t="s">
-        <v>159</v>
+      <c r="D128" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="E128" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" s="6"/>
       <c r="C129" s="6" t="s">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="D129" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" s="6"/>
       <c r="D130" s="6" t="s">
-        <v>305</v>
+        <v>285</v>
       </c>
       <c r="E130" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" s="6"/>
       <c r="D131" s="6" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="E131" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C132" t="s">
-        <v>162</v>
+      <c r="B132" s="6"/>
+      <c r="D132" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E132" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" s="6"/>
-      <c r="C133" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D133" t="s">
-        <v>167</v>
+      <c r="D133" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E133" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" s="6"/>
-      <c r="C134" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="D134" t="s">
-        <v>168</v>
+      <c r="D134" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E134" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" s="6"/>
       <c r="C135" s="6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="D135" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
     </row>
     <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" s="6"/>
-      <c r="C136" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="D136" t="s">
-        <v>171</v>
+      <c r="D136" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E136" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C137" t="s">
-        <v>163</v>
+      <c r="B137" s="6"/>
+      <c r="D137" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="E137" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="138" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B138" s="6"/>
-      <c r="C138" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D138" t="s">
-        <v>170</v>
+      <c r="B138" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="C138" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B139" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C139" t="s">
-        <v>164</v>
+      <c r="B139" s="6"/>
+      <c r="C139" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D139" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" s="6"/>
       <c r="C140" s="6" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="D140" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
     </row>
     <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" s="6"/>
-      <c r="C141" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="D141" t="s">
-        <v>165</v>
+      <c r="D141" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E141" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" s="6"/>
-      <c r="C142" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="D142" t="s">
-        <v>166</v>
+      <c r="D142" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E142" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" s="6" t="s">
-        <v>318</v>
+        <v>298</v>
       </c>
       <c r="C143" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" s="6"/>
       <c r="C144" s="6" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="D144" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B145" s="6"/>
       <c r="C145" s="6" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="D145" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B146" s="6"/>
       <c r="C146" s="6" t="s">
-        <v>320</v>
+        <v>301</v>
       </c>
       <c r="D146" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B147" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="C147" t="s">
-        <v>173</v>
+      <c r="B147" s="6"/>
+      <c r="C147" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="D147" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="148" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B148" s="6"/>
-      <c r="C148" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="D148" t="s">
-        <v>174</v>
+      <c r="B148" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C148" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="149" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
       <c r="C149" s="6" t="s">
-        <v>323</v>
+        <v>304</v>
       </c>
       <c r="D149" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="150" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B150" s="6"/>
-      <c r="C150" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="D150" t="s">
-        <v>176</v>
+      <c r="B150" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="C150" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B151" s="6"/>
+      <c r="C151" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="D151" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B152" s="6"/>
+      <c r="C152" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="D152" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B153" s="6"/>
+      <c r="C153" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D153" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B154" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C154" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B155" s="6"/>
+      <c r="C155" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D155" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B156" s="6"/>
+      <c r="C156" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D156" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B157" s="6"/>
+      <c r="C157" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D157" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B158" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C158" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="6"/>
+      <c r="C159" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D159" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B160" s="6"/>
+      <c r="C160" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D160" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B161" s="6"/>
+      <c r="C161" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D161" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J28" r:id="rId1" xr:uid="{970CC680-CF0D-4561-AC7A-E5895C962FED}"/>
-    <hyperlink ref="J37" r:id="rId2" xr:uid="{E9039A44-B60A-4B1D-BDFD-D798781C1619}"/>
-    <hyperlink ref="J54" r:id="rId3" xr:uid="{1D969E3C-7E19-4FED-8815-5B572A9C997E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2 A75" numberStoredAsText="1"/>
+    <ignoredError sqref="A2 A86" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2769,7 +3315,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2791,12 +3337,12 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2806,7 +3352,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2816,7 +3362,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2826,300 +3372,300 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="I18" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="O26" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="W27" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="W28" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="I29" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="W29" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="I35" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="I42" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="L56" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="M57" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="M58" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="N59" t="s">
         <v>2</v>
@@ -3127,15 +3673,15 @@
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="M60" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="N61" t="s">
         <v>2</v>
@@ -3143,92 +3689,92 @@
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C79" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>